<commit_message>
Updated Invoice template format
</commit_message>
<xml_diff>
--- a/Documents/InvoiceTemplates/standardInvoice.xlsx
+++ b/Documents/InvoiceTemplates/standardInvoice.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Invoice" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Invoice!$J$8:$J$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Invoice!$J$6:$J$28</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -339,6 +339,35 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -349,35 +378,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -751,10 +751,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M87"/>
+  <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:L5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -772,137 +772,171 @@
     <row r="1" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-    </row>
-    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+    </row>
+    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="44"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+    </row>
+    <row r="8" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+    </row>
+    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="42" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="41"/>
       <c r="B9" s="41"/>
       <c r="C9" s="41"/>
       <c r="D9" s="41"/>
       <c r="E9" s="41"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-    </row>
-    <row r="10" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="41"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="12">
+        <f t="shared" ref="I9:I48" si="0">G9*H9</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1" t="str">
+        <f t="shared" ref="J9:J28" si="1">IF(I9&gt;0,I9," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>2</v>
+      </c>
       <c r="B10" s="41"/>
       <c r="C10" s="41"/>
       <c r="D10" s="41"/>
       <c r="E10" s="41"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
-        <v>1</v>
-      </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
+        <v>3</v>
+      </c>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="10"/>
+      <c r="G11" s="13"/>
       <c r="H11" s="11"/>
       <c r="I11" s="12">
-        <f t="shared" ref="I11:I52" si="0">G11*H11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J11" s="1" t="str">
-        <f t="shared" ref="J11:J30" si="1">IF(I11&gt;0,I11," ")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
-        <v>2</v>
-      </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
+        <v>4</v>
+      </c>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="9"/>
       <c r="G12" s="13"/>
       <c r="H12" s="11"/>
@@ -917,12 +951,12 @@
     </row>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
-        <v>3</v>
-      </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
+        <v>5</v>
+      </c>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
       <c r="F13" s="9"/>
       <c r="G13" s="13"/>
       <c r="H13" s="11"/>
@@ -937,12 +971,12 @@
     </row>
     <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
-        <v>4</v>
-      </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
+        <v>6</v>
+      </c>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
       <c r="F14" s="9"/>
       <c r="G14" s="13"/>
       <c r="H14" s="11"/>
@@ -957,12 +991,12 @@
     </row>
     <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
-        <v>5</v>
-      </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
+        <v>7</v>
+      </c>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
       <c r="F15" s="9"/>
       <c r="G15" s="13"/>
       <c r="H15" s="11"/>
@@ -977,12 +1011,12 @@
     </row>
     <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
-        <v>6</v>
-      </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
+        <v>8</v>
+      </c>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
       <c r="F16" s="9"/>
       <c r="G16" s="13"/>
       <c r="H16" s="11"/>
@@ -997,12 +1031,12 @@
     </row>
     <row r="17" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
-        <v>7</v>
-      </c>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
+        <v>9</v>
+      </c>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
       <c r="F17" s="9"/>
       <c r="G17" s="13"/>
       <c r="H17" s="11"/>
@@ -1017,14 +1051,14 @@
     </row>
     <row r="18" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
-        <v>8</v>
-      </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
+        <v>10</v>
+      </c>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="13"/>
+      <c r="G18" s="8"/>
       <c r="H18" s="11"/>
       <c r="I18" s="12">
         <f t="shared" si="0"/>
@@ -1037,14 +1071,14 @@
     </row>
     <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
-        <v>9</v>
-      </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
+        <v>11</v>
+      </c>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
       <c r="F19" s="9"/>
-      <c r="G19" s="13"/>
+      <c r="G19" s="8"/>
       <c r="H19" s="11"/>
       <c r="I19" s="12">
         <f t="shared" si="0"/>
@@ -1057,12 +1091,12 @@
     </row>
     <row r="20" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
-        <v>10</v>
-      </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
+        <v>12</v>
+      </c>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
       <c r="F20" s="9"/>
       <c r="G20" s="8"/>
       <c r="H20" s="11"/>
@@ -1077,12 +1111,12 @@
     </row>
     <row r="21" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
-        <v>11</v>
-      </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
+        <v>13</v>
+      </c>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
       <c r="F21" s="9"/>
       <c r="G21" s="8"/>
       <c r="H21" s="11"/>
@@ -1097,12 +1131,12 @@
     </row>
     <row r="22" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
-        <v>12</v>
-      </c>
-      <c r="B22" s="44"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
+        <v>14</v>
+      </c>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
       <c r="F22" s="9"/>
       <c r="G22" s="8"/>
       <c r="H22" s="11"/>
@@ -1115,18 +1149,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <v>13</v>
-      </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
+        <v>15</v>
+      </c>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="12">
+      <c r="G23" s="14"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1135,18 +1169,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <v>14</v>
-      </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
+        <v>16</v>
+      </c>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="12">
+      <c r="G24" s="14"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1157,12 +1191,12 @@
     </row>
     <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <v>15</v>
-      </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
+        <v>17</v>
+      </c>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
       <c r="F25" s="9"/>
       <c r="G25" s="14"/>
       <c r="H25" s="15"/>
@@ -1177,12 +1211,12 @@
     </row>
     <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
-        <v>16</v>
-      </c>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
+        <v>18</v>
+      </c>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
       <c r="F26" s="9"/>
       <c r="G26" s="14"/>
       <c r="H26" s="15"/>
@@ -1197,12 +1231,12 @@
     </row>
     <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
-        <v>17</v>
-      </c>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
+        <v>19</v>
+      </c>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
       <c r="F27" s="9"/>
       <c r="G27" s="14"/>
       <c r="H27" s="15"/>
@@ -1217,12 +1251,12 @@
     </row>
     <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
-        <v>18</v>
-      </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
+        <v>20</v>
+      </c>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
       <c r="F28" s="9"/>
       <c r="G28" s="14"/>
       <c r="H28" s="15"/>
@@ -1237,12 +1271,12 @@
     </row>
     <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
-        <v>19</v>
-      </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
+        <v>21</v>
+      </c>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
       <c r="F29" s="9"/>
       <c r="G29" s="14"/>
       <c r="H29" s="15"/>
@@ -1250,19 +1284,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J29" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
     </row>
     <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
-        <v>20</v>
-      </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
+        <v>22</v>
+      </c>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
       <c r="F30" s="9"/>
       <c r="G30" s="14"/>
       <c r="H30" s="15"/>
@@ -1270,19 +1300,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J30" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
     </row>
     <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
-        <v>21</v>
-      </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
+        <v>23</v>
+      </c>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
       <c r="F31" s="9"/>
       <c r="G31" s="14"/>
       <c r="H31" s="15"/>
@@ -1293,12 +1319,12 @@
     </row>
     <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
-        <v>22</v>
-      </c>
-      <c r="B32" s="45"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
+        <v>24</v>
+      </c>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
       <c r="F32" s="9"/>
       <c r="G32" s="14"/>
       <c r="H32" s="15"/>
@@ -1309,12 +1335,12 @@
     </row>
     <row r="33" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
-        <v>23</v>
-      </c>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
+        <v>25</v>
+      </c>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
       <c r="F33" s="9"/>
       <c r="G33" s="14"/>
       <c r="H33" s="15"/>
@@ -1325,12 +1351,12 @@
     </row>
     <row r="34" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
-        <v>24</v>
-      </c>
-      <c r="B34" s="45"/>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
+        <v>26</v>
+      </c>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
       <c r="F34" s="9"/>
       <c r="G34" s="14"/>
       <c r="H34" s="15"/>
@@ -1341,12 +1367,12 @@
     </row>
     <row r="35" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
-        <v>25</v>
-      </c>
-      <c r="B35" s="45"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
+        <v>27</v>
+      </c>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
       <c r="F35" s="9"/>
       <c r="G35" s="14"/>
       <c r="H35" s="15"/>
@@ -1357,12 +1383,12 @@
     </row>
     <row r="36" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
-        <v>26</v>
-      </c>
-      <c r="B36" s="45"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
+        <v>28</v>
+      </c>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
       <c r="F36" s="9"/>
       <c r="G36" s="14"/>
       <c r="H36" s="15"/>
@@ -1373,12 +1399,12 @@
     </row>
     <row r="37" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
-        <v>27</v>
-      </c>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
+        <v>29</v>
+      </c>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
       <c r="F37" s="9"/>
       <c r="G37" s="14"/>
       <c r="H37" s="15"/>
@@ -1389,12 +1415,12 @@
     </row>
     <row r="38" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
-        <v>28</v>
-      </c>
-      <c r="B38" s="45"/>
-      <c r="C38" s="45"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="45"/>
+        <v>30</v>
+      </c>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="9"/>
       <c r="G38" s="14"/>
       <c r="H38" s="15"/>
@@ -1405,12 +1431,12 @@
     </row>
     <row r="39" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
-        <v>29</v>
-      </c>
-      <c r="B39" s="45"/>
-      <c r="C39" s="45"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="45"/>
+        <v>31</v>
+      </c>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
       <c r="F39" s="9"/>
       <c r="G39" s="14"/>
       <c r="H39" s="15"/>
@@ -1421,12 +1447,12 @@
     </row>
     <row r="40" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
-        <v>30</v>
-      </c>
-      <c r="B40" s="45"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
+        <v>32</v>
+      </c>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
       <c r="F40" s="9"/>
       <c r="G40" s="14"/>
       <c r="H40" s="15"/>
@@ -1437,12 +1463,12 @@
     </row>
     <row r="41" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
-        <v>31</v>
-      </c>
-      <c r="B41" s="45"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
+        <v>33</v>
+      </c>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
       <c r="F41" s="9"/>
       <c r="G41" s="14"/>
       <c r="H41" s="15"/>
@@ -1453,12 +1479,12 @@
     </row>
     <row r="42" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
-        <v>32</v>
-      </c>
-      <c r="B42" s="45"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45"/>
+        <v>34</v>
+      </c>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
       <c r="F42" s="9"/>
       <c r="G42" s="14"/>
       <c r="H42" s="15"/>
@@ -1469,12 +1495,12 @@
     </row>
     <row r="43" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
-        <v>33</v>
-      </c>
-      <c r="B43" s="45"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
+        <v>35</v>
+      </c>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
       <c r="F43" s="9"/>
       <c r="G43" s="14"/>
       <c r="H43" s="15"/>
@@ -1485,12 +1511,12 @@
     </row>
     <row r="44" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
-        <v>34</v>
-      </c>
-      <c r="B44" s="45"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="45"/>
+        <v>36</v>
+      </c>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
       <c r="F44" s="9"/>
       <c r="G44" s="14"/>
       <c r="H44" s="15"/>
@@ -1501,12 +1527,12 @@
     </row>
     <row r="45" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
-        <v>35</v>
-      </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
+        <v>37</v>
+      </c>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
       <c r="F45" s="9"/>
       <c r="G45" s="14"/>
       <c r="H45" s="15"/>
@@ -1517,12 +1543,12 @@
     </row>
     <row r="46" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
-        <v>36</v>
-      </c>
-      <c r="B46" s="45"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
+        <v>38</v>
+      </c>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
       <c r="F46" s="9"/>
       <c r="G46" s="14"/>
       <c r="H46" s="15"/>
@@ -1533,12 +1559,12 @@
     </row>
     <row r="47" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
-        <v>37</v>
-      </c>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
+        <v>39</v>
+      </c>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
       <c r="F47" s="9"/>
       <c r="G47" s="14"/>
       <c r="H47" s="15"/>
@@ -1549,12 +1575,12 @@
     </row>
     <row r="48" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
-        <v>38</v>
-      </c>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
+        <v>40</v>
+      </c>
+      <c r="B48" s="38"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="38"/>
       <c r="F48" s="9"/>
       <c r="G48" s="14"/>
       <c r="H48" s="15"/>
@@ -1563,168 +1589,148 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="8">
-        <v>39</v>
-      </c>
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="15"/>
+    <row r="49" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" s="39"/>
       <c r="I49" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="8">
-        <v>40</v>
-      </c>
-      <c r="B50" s="45"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="15"/>
-      <c r="I50" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="8">
-        <v>41</v>
-      </c>
-      <c r="B51" s="45"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="15"/>
-      <c r="I51" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="8">
-        <v>42</v>
-      </c>
-      <c r="B52" s="45"/>
-      <c r="C52" s="45"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="45"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="H53" s="47"/>
-      <c r="I53" s="16">
-        <f>SUM(I11:I52)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
-      <c r="J54" s="19"/>
-    </row>
-    <row r="55" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A55" s="20"/>
-      <c r="B55" s="46" t="s">
+        <f>SUM(I9:I48)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="20"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="19"/>
+    </row>
+    <row r="51" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A51" s="20"/>
+      <c r="B51" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C55" s="46"/>
-      <c r="D55" s="46"/>
-      <c r="E55" s="46"/>
-      <c r="F55" s="46"/>
-      <c r="G55" s="46" t="s">
+      <c r="C51" s="37"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="H55" s="46"/>
-      <c r="I55" s="46"/>
-      <c r="J55" s="19"/>
-    </row>
-    <row r="56" spans="1:10" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A56" s="21"/>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="22"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="22"/>
-      <c r="G56" s="23"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="21"/>
-    </row>
-    <row r="57" spans="1:10" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A57" s="21"/>
-      <c r="B57" s="21"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="22"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="22"/>
-      <c r="G57" s="23"/>
-      <c r="H57" s="21"/>
-      <c r="I57" s="21"/>
-    </row>
-    <row r="58" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A58" s="24"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="26"/>
-      <c r="H58" s="24"/>
-      <c r="I58" s="24"/>
-    </row>
-    <row r="59" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A59" s="27"/>
-      <c r="B59" s="27"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="27"/>
-      <c r="H59" s="27"/>
-      <c r="I59" s="27"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="37"/>
+      <c r="J51" s="19"/>
+    </row>
+    <row r="52" spans="1:10" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+    </row>
+    <row r="53" spans="1:10" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A53" s="21"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="23"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+    </row>
+    <row r="54" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A54" s="24"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="24"/>
+    </row>
+    <row r="55" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="A55" s="27"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="27"/>
+      <c r="I55" s="27"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="28"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="28"/>
+      <c r="I56" s="28"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="29"/>
+      <c r="B57" s="29"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="29"/>
+      <c r="H57" s="29"/>
+      <c r="I57" s="29"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="30"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="30"/>
+      <c r="G58" s="30"/>
+      <c r="H58" s="30"/>
+      <c r="I58" s="30"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="29"/>
+      <c r="B59" s="29"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
+      <c r="G59" s="29"/>
+      <c r="H59" s="29"/>
+      <c r="I59" s="29"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A60" s="28"/>
-      <c r="B60" s="28"/>
-      <c r="C60" s="28"/>
-      <c r="D60" s="28"/>
-      <c r="E60" s="28"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="28"/>
-      <c r="H60" s="28"/>
-      <c r="I60" s="28"/>
+      <c r="A60" s="30"/>
+      <c r="B60" s="30"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="30"/>
+      <c r="G60" s="30"/>
+      <c r="H60" s="30"/>
+      <c r="I60" s="30"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="29"/>
@@ -1781,71 +1787,71 @@
       <c r="H65" s="29"/>
       <c r="I65" s="29"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="30"/>
-      <c r="B66" s="30"/>
-      <c r="C66" s="30"/>
-      <c r="D66" s="30"/>
-      <c r="E66" s="30"/>
-      <c r="F66" s="30"/>
-      <c r="G66" s="30"/>
-      <c r="H66" s="30"/>
-      <c r="I66" s="30"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="29"/>
-      <c r="B67" s="29"/>
-      <c r="C67" s="29"/>
-      <c r="D67" s="29"/>
-      <c r="E67" s="29"/>
-      <c r="F67" s="29"/>
-      <c r="G67" s="29"/>
-      <c r="H67" s="29"/>
-      <c r="I67" s="29"/>
+    <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A66" s="31"/>
+      <c r="B66" s="31"/>
+      <c r="C66" s="31"/>
+      <c r="D66" s="31"/>
+      <c r="E66" s="31"/>
+      <c r="F66" s="31"/>
+      <c r="G66" s="31"/>
+      <c r="H66" s="31"/>
+      <c r="I66" s="31"/>
+    </row>
+    <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A67" s="31"/>
+      <c r="B67" s="31"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="31"/>
+      <c r="F67" s="31"/>
+      <c r="G67" s="31"/>
+      <c r="H67" s="31"/>
+      <c r="I67" s="31"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="30"/>
-      <c r="B68" s="30"/>
-      <c r="C68" s="30"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="30"/>
-      <c r="F68" s="30"/>
-      <c r="G68" s="30"/>
-      <c r="H68" s="30"/>
-      <c r="I68" s="30"/>
+      <c r="A68" s="32"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="33"/>
+      <c r="D68" s="33"/>
+      <c r="E68" s="33"/>
+      <c r="F68" s="33"/>
+      <c r="G68" s="32"/>
+      <c r="H68" s="32"/>
+      <c r="I68" s="34"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="29"/>
-      <c r="B69" s="29"/>
-      <c r="C69" s="29"/>
-      <c r="D69" s="29"/>
-      <c r="E69" s="29"/>
-      <c r="F69" s="29"/>
-      <c r="G69" s="29"/>
-      <c r="H69" s="29"/>
-      <c r="I69" s="29"/>
-    </row>
-    <row r="70" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A70" s="31"/>
-      <c r="B70" s="31"/>
-      <c r="C70" s="31"/>
-      <c r="D70" s="31"/>
-      <c r="E70" s="31"/>
-      <c r="F70" s="31"/>
-      <c r="G70" s="31"/>
-      <c r="H70" s="31"/>
-      <c r="I70" s="31"/>
-    </row>
-    <row r="71" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A71" s="31"/>
-      <c r="B71" s="31"/>
-      <c r="C71" s="31"/>
-      <c r="D71" s="31"/>
-      <c r="E71" s="31"/>
-      <c r="F71" s="31"/>
-      <c r="G71" s="31"/>
-      <c r="H71" s="31"/>
-      <c r="I71" s="31"/>
+      <c r="A69" s="32"/>
+      <c r="B69" s="33"/>
+      <c r="C69" s="33"/>
+      <c r="D69" s="33"/>
+      <c r="E69" s="33"/>
+      <c r="F69" s="33"/>
+      <c r="G69" s="32"/>
+      <c r="H69" s="32"/>
+      <c r="I69" s="34"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="32"/>
+      <c r="B70" s="33"/>
+      <c r="C70" s="33"/>
+      <c r="D70" s="33"/>
+      <c r="E70" s="33"/>
+      <c r="F70" s="33"/>
+      <c r="G70" s="32"/>
+      <c r="H70" s="32"/>
+      <c r="I70" s="34"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="32"/>
+      <c r="B71" s="33"/>
+      <c r="C71" s="33"/>
+      <c r="D71" s="33"/>
+      <c r="E71" s="33"/>
+      <c r="F71" s="33"/>
+      <c r="G71" s="32"/>
+      <c r="H71" s="32"/>
+      <c r="I71" s="34"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="32"/>
@@ -1948,141 +1954,94 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="32"/>
-      <c r="B81" s="33"/>
-      <c r="C81" s="33"/>
-      <c r="D81" s="33"/>
-      <c r="E81" s="33"/>
-      <c r="F81" s="33"/>
-      <c r="G81" s="32"/>
-      <c r="H81" s="32"/>
+      <c r="B81" s="32"/>
+      <c r="C81" s="32"/>
+      <c r="D81" s="32"/>
+      <c r="E81" s="32"/>
+      <c r="F81" s="35"/>
+      <c r="G81" s="35"/>
+      <c r="H81" s="33"/>
       <c r="I81" s="34"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="32"/>
-      <c r="B82" s="33"/>
-      <c r="C82" s="33"/>
-      <c r="D82" s="33"/>
-      <c r="E82" s="33"/>
-      <c r="F82" s="33"/>
-      <c r="G82" s="32"/>
-      <c r="H82" s="32"/>
+      <c r="B82" s="32"/>
+      <c r="C82" s="32"/>
+      <c r="D82" s="32"/>
+      <c r="E82" s="32"/>
+      <c r="F82" s="35"/>
+      <c r="G82" s="35"/>
+      <c r="H82" s="33"/>
       <c r="I82" s="34"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="32"/>
-      <c r="B83" s="33"/>
-      <c r="C83" s="33"/>
-      <c r="D83" s="33"/>
-      <c r="E83" s="33"/>
-      <c r="F83" s="33"/>
-      <c r="G83" s="32"/>
-      <c r="H83" s="32"/>
+      <c r="B83" s="32"/>
+      <c r="C83" s="32"/>
+      <c r="D83" s="32"/>
+      <c r="E83" s="32"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="35"/>
+      <c r="H83" s="33"/>
       <c r="I83" s="34"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" s="32"/>
-      <c r="B84" s="33"/>
-      <c r="C84" s="33"/>
-      <c r="D84" s="33"/>
-      <c r="E84" s="33"/>
-      <c r="F84" s="33"/>
-      <c r="G84" s="32"/>
-      <c r="H84" s="32"/>
-      <c r="I84" s="34"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" s="32"/>
-      <c r="B85" s="32"/>
-      <c r="C85" s="32"/>
-      <c r="D85" s="32"/>
-      <c r="E85" s="32"/>
-      <c r="F85" s="35"/>
-      <c r="G85" s="35"/>
-      <c r="H85" s="33"/>
-      <c r="I85" s="34"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" s="32"/>
-      <c r="B86" s="32"/>
-      <c r="C86" s="32"/>
-      <c r="D86" s="32"/>
-      <c r="E86" s="32"/>
-      <c r="F86" s="35"/>
-      <c r="G86" s="35"/>
-      <c r="H86" s="33"/>
-      <c r="I86" s="34"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87" s="32"/>
-      <c r="B87" s="32"/>
-      <c r="C87" s="32"/>
-      <c r="D87" s="32"/>
-      <c r="E87" s="32"/>
-      <c r="F87" s="35"/>
-      <c r="G87" s="35"/>
-      <c r="H87" s="33"/>
-      <c r="I87" s="34"/>
-    </row>
   </sheetData>
-  <autoFilter ref="J8:J30"/>
-  <mergeCells count="57">
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="G55:I55"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B48:E48"/>
+  <mergeCells count="55">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:E8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:E38"/>
     <mergeCell ref="B39:E39"/>
     <mergeCell ref="B40:E40"/>
     <mergeCell ref="B41:E41"/>
     <mergeCell ref="B42:E42"/>
     <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="G49:H49"/>
   </mergeCells>
   <pageMargins left="0.390277777777778" right="0.15" top="0.30972222222222201" bottom="0.25972222222222202" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated XLS template sheet according to reqiurements
</commit_message>
<xml_diff>
--- a/Documents/InvoiceTemplates/standardInvoice.xlsx
+++ b/Documents/InvoiceTemplates/standardInvoice.xlsx
@@ -17,16 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Постачальник</t>
-  </si>
-  <si>
-    <t>Одержувач</t>
-  </si>
-  <si>
-    <t>Видаткова накладна №</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>від "     " _____________  200_ р.</t>
   </si>
@@ -43,12 +34,6 @@
     <t>Кількість</t>
   </si>
   <si>
-    <t>Відвантажив(ла)______________________</t>
-  </si>
-  <si>
-    <t>Отримав(ла) ______________________________</t>
-  </si>
-  <si>
     <t>Ціна</t>
   </si>
   <si>
@@ -56,6 +41,18 @@
   </si>
   <si>
     <t>Разом:</t>
+  </si>
+  <si>
+    <t>НАКЛАДНА №</t>
+  </si>
+  <si>
+    <t>Кому відпущено</t>
+  </si>
+  <si>
+    <t>Відпустив______________________</t>
+  </si>
+  <si>
+    <t>Отримав _____________________</t>
   </si>
 </sst>
 </file>
@@ -216,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -338,6 +335,18 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
@@ -360,10 +369,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -373,10 +378,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -754,7 +755,7 @@
   <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+      <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -769,825 +770,554 @@
     <col min="10" max="10" width="12.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="45" t="s">
+    <row r="2" spans="1:10" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-    </row>
-    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="45" t="s">
-        <v>1</v>
+      <c r="B3" s="4"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="47" t="s">
+        <v>9</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="47" t="s">
-        <v>2</v>
-      </c>
+      <c r="C4" s="47"/>
       <c r="D4" s="47"/>
       <c r="E4" s="47"/>
       <c r="F4" s="47"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+    </row>
+    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="43" t="s">
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+    </row>
+    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="44" t="s">
+      <c r="G6" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="H6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="42" t="s">
+      <c r="I6" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="42" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="7" spans="1:10" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="44"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
     </row>
     <row r="8" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="44"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
     </row>
     <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
-        <v>1</v>
-      </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
       <c r="F9" s="9"/>
       <c r="G9" s="10"/>
       <c r="H9" s="11"/>
-      <c r="I9" s="12">
-        <f t="shared" ref="I9:I48" si="0">G9*H9</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="1" t="str">
-        <f t="shared" ref="J9:J28" si="1">IF(I9&gt;0,I9," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
-        <v>2</v>
-      </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
       <c r="F10" s="9"/>
       <c r="G10" s="13"/>
       <c r="H10" s="11"/>
-      <c r="I10" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="I10" s="12"/>
     </row>
     <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
-        <v>3</v>
-      </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="9"/>
       <c r="G11" s="13"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="I11" s="12"/>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
-        <v>4</v>
-      </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="9"/>
       <c r="G12" s="13"/>
       <c r="H12" s="11"/>
-      <c r="I12" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="I12" s="12"/>
     </row>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
-        <v>5</v>
-      </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
       <c r="F13" s="9"/>
       <c r="G13" s="13"/>
       <c r="H13" s="11"/>
-      <c r="I13" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
-        <v>6</v>
-      </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
       <c r="F14" s="9"/>
       <c r="G14" s="13"/>
       <c r="H14" s="11"/>
-      <c r="I14" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="I14" s="12"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8">
-        <v>7</v>
-      </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
       <c r="F15" s="9"/>
       <c r="G15" s="13"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="8">
-        <v>8</v>
-      </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
       <c r="F16" s="9"/>
       <c r="G16" s="13"/>
       <c r="H16" s="11"/>
-      <c r="I16" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="8">
-        <v>9</v>
-      </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
       <c r="F17" s="9"/>
       <c r="G17" s="13"/>
       <c r="H17" s="11"/>
-      <c r="I17" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="8">
-        <v>10</v>
-      </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
       <c r="F18" s="9"/>
       <c r="G18" s="8"/>
       <c r="H18" s="11"/>
-      <c r="I18" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="8">
-        <v>11</v>
-      </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
       <c r="F19" s="9"/>
       <c r="G19" s="8"/>
       <c r="H19" s="11"/>
-      <c r="I19" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="8">
-        <v>12</v>
-      </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
       <c r="F20" s="9"/>
       <c r="G20" s="8"/>
       <c r="H20" s="11"/>
-      <c r="I20" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="8">
-        <v>13</v>
-      </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
       <c r="F21" s="9"/>
       <c r="G21" s="8"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="8">
-        <v>14</v>
-      </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
       <c r="F22" s="9"/>
       <c r="G22" s="8"/>
       <c r="H22" s="11"/>
-      <c r="I22" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
-        <v>15</v>
-      </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
       <c r="F23" s="9"/>
       <c r="G23" s="14"/>
       <c r="H23" s="15"/>
-      <c r="I23" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
-        <v>16</v>
-      </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
+      <c r="I23" s="16"/>
+    </row>
+    <row r="24" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
       <c r="F24" s="9"/>
       <c r="G24" s="14"/>
       <c r="H24" s="15"/>
-      <c r="I24" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
-        <v>17</v>
-      </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
       <c r="F25" s="9"/>
       <c r="G25" s="14"/>
       <c r="H25" s="15"/>
-      <c r="I25" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
-        <v>18</v>
-      </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
+      <c r="I25" s="16"/>
+    </row>
+    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
       <c r="F26" s="9"/>
       <c r="G26" s="14"/>
       <c r="H26" s="15"/>
-      <c r="I26" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J26" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
-        <v>19</v>
-      </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
+      <c r="I26" s="16"/>
+    </row>
+    <row r="27" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
       <c r="F27" s="9"/>
       <c r="G27" s="14"/>
       <c r="H27" s="15"/>
-      <c r="I27" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J27" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
-        <v>20</v>
-      </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
+      <c r="I27" s="16"/>
+    </row>
+    <row r="28" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
       <c r="F28" s="9"/>
       <c r="G28" s="14"/>
       <c r="H28" s="15"/>
-      <c r="I28" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J28" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8">
-        <v>21</v>
-      </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
+      <c r="I28" s="16"/>
+    </row>
+    <row r="29" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
       <c r="F29" s="9"/>
       <c r="G29" s="14"/>
       <c r="H29" s="15"/>
-      <c r="I29" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
-        <v>22</v>
-      </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
+      <c r="I29" s="16"/>
+    </row>
+    <row r="30" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
       <c r="F30" s="9"/>
       <c r="G30" s="14"/>
       <c r="H30" s="15"/>
-      <c r="I30" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
-        <v>23</v>
-      </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
+      <c r="I30" s="16"/>
+    </row>
+    <row r="31" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
       <c r="F31" s="9"/>
       <c r="G31" s="14"/>
       <c r="H31" s="15"/>
-      <c r="I31" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
-        <v>24</v>
-      </c>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
+      <c r="I31" s="16"/>
+    </row>
+    <row r="32" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
       <c r="F32" s="9"/>
       <c r="G32" s="14"/>
       <c r="H32" s="15"/>
-      <c r="I32" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I32" s="16"/>
     </row>
     <row r="33" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
-        <v>25</v>
-      </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
       <c r="F33" s="9"/>
       <c r="G33" s="14"/>
       <c r="H33" s="15"/>
-      <c r="I33" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I33" s="16"/>
     </row>
     <row r="34" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
-        <v>26</v>
-      </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
       <c r="F34" s="9"/>
       <c r="G34" s="14"/>
       <c r="H34" s="15"/>
-      <c r="I34" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I34" s="16"/>
     </row>
     <row r="35" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8">
-        <v>27</v>
-      </c>
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
+      <c r="A35" s="8"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
       <c r="F35" s="9"/>
       <c r="G35" s="14"/>
       <c r="H35" s="15"/>
-      <c r="I35" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I35" s="16"/>
     </row>
     <row r="36" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="8">
-        <v>28</v>
-      </c>
-      <c r="B36" s="38"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="41"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="41"/>
       <c r="F36" s="9"/>
       <c r="G36" s="14"/>
       <c r="H36" s="15"/>
-      <c r="I36" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I36" s="16"/>
     </row>
     <row r="37" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8">
-        <v>29</v>
-      </c>
-      <c r="B37" s="38"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
       <c r="F37" s="9"/>
       <c r="G37" s="14"/>
       <c r="H37" s="15"/>
-      <c r="I37" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I37" s="16"/>
     </row>
     <row r="38" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
-        <v>30</v>
-      </c>
-      <c r="B38" s="38"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
       <c r="F38" s="9"/>
       <c r="G38" s="14"/>
       <c r="H38" s="15"/>
-      <c r="I38" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I38" s="16"/>
     </row>
     <row r="39" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8">
-        <v>31</v>
-      </c>
-      <c r="B39" s="38"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="41"/>
       <c r="F39" s="9"/>
       <c r="G39" s="14"/>
       <c r="H39" s="15"/>
-      <c r="I39" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I39" s="16"/>
     </row>
     <row r="40" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="8">
-        <v>32</v>
-      </c>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="41"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="41"/>
       <c r="F40" s="9"/>
       <c r="G40" s="14"/>
       <c r="H40" s="15"/>
-      <c r="I40" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I40" s="16"/>
     </row>
     <row r="41" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8">
-        <v>33</v>
-      </c>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="41"/>
       <c r="F41" s="9"/>
       <c r="G41" s="14"/>
       <c r="H41" s="15"/>
-      <c r="I41" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I41" s="16"/>
     </row>
     <row r="42" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="8">
-        <v>34</v>
-      </c>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="41"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="41"/>
+      <c r="E42" s="41"/>
       <c r="F42" s="9"/>
       <c r="G42" s="14"/>
       <c r="H42" s="15"/>
-      <c r="I42" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I42" s="16"/>
     </row>
     <row r="43" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="8">
-        <v>35</v>
-      </c>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
+      <c r="A43" s="8"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="41"/>
       <c r="F43" s="9"/>
       <c r="G43" s="14"/>
       <c r="H43" s="15"/>
-      <c r="I43" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I43" s="16"/>
     </row>
     <row r="44" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="8">
-        <v>36</v>
-      </c>
-      <c r="B44" s="38"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="41"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="41"/>
       <c r="F44" s="9"/>
       <c r="G44" s="14"/>
       <c r="H44" s="15"/>
-      <c r="I44" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I44" s="16"/>
     </row>
     <row r="45" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="8">
-        <v>37</v>
-      </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="41"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="41"/>
+      <c r="E45" s="41"/>
       <c r="F45" s="9"/>
       <c r="G45" s="14"/>
       <c r="H45" s="15"/>
-      <c r="I45" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I45" s="16"/>
     </row>
     <row r="46" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="8">
-        <v>38</v>
-      </c>
-      <c r="B46" s="38"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="41"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="41"/>
+      <c r="E46" s="41"/>
       <c r="F46" s="9"/>
       <c r="G46" s="14"/>
       <c r="H46" s="15"/>
-      <c r="I46" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I46" s="16"/>
     </row>
     <row r="47" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="8">
-        <v>39</v>
-      </c>
-      <c r="B47" s="38"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
+      <c r="A47" s="8"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
       <c r="F47" s="9"/>
       <c r="G47" s="14"/>
       <c r="H47" s="15"/>
-      <c r="I47" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I47" s="16"/>
     </row>
     <row r="48" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="8">
-        <v>40</v>
-      </c>
-      <c r="B48" s="38"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="38"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="41"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="41"/>
       <c r="F48" s="9"/>
       <c r="G48" s="14"/>
       <c r="H48" s="15"/>
-      <c r="I48" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I48" s="16"/>
     </row>
     <row r="49" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
@@ -1596,10 +1326,10 @@
       <c r="D49" s="17"/>
       <c r="E49" s="17"/>
       <c r="F49" s="18"/>
-      <c r="G49" s="39" t="s">
-        <v>12</v>
+      <c r="G49" s="42" t="s">
+        <v>7</v>
       </c>
-      <c r="H49" s="39"/>
+      <c r="H49" s="42"/>
       <c r="I49" s="16">
         <f>SUM(I9:I48)</f>
         <v>0</v>
@@ -1619,18 +1349,18 @@
     </row>
     <row r="51" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A51" s="20"/>
-      <c r="B51" s="37" t="s">
-        <v>8</v>
+      <c r="B51" s="40" t="s">
+        <v>10</v>
       </c>
-      <c r="C51" s="37"/>
-      <c r="D51" s="37"/>
-      <c r="E51" s="37"/>
-      <c r="F51" s="37"/>
-      <c r="G51" s="37" t="s">
-        <v>9</v>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="40" t="s">
+        <v>11</v>
       </c>
-      <c r="H51" s="37"/>
-      <c r="I51" s="37"/>
+      <c r="H51" s="40"/>
+      <c r="I51" s="40"/>
       <c r="J51" s="19"/>
     </row>
     <row r="52" spans="1:10" ht="20.25" x14ac:dyDescent="0.2">
@@ -1987,16 +1717,14 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:I4"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:E8"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="G6:G8"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:I5"/>
     <mergeCell ref="H6:H8"/>
     <mergeCell ref="I6:I8"/>
     <mergeCell ref="B9:E9"/>
@@ -2022,26 +1750,28 @@
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B41:E41"/>
     <mergeCell ref="B32:E32"/>
     <mergeCell ref="B33:E33"/>
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="B35:E35"/>
     <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="G49:H49"/>
     <mergeCell ref="B42:E42"/>
     <mergeCell ref="B43:E43"/>
     <mergeCell ref="B44:E44"/>
     <mergeCell ref="B45:E45"/>
     <mergeCell ref="B46:E46"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B40:E40"/>
   </mergeCells>
   <pageMargins left="0.390277777777778" right="0.15" top="0.30972222222222201" bottom="0.25972222222222202" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>